<commit_message>
add the name of the user logging on to the report
</commit_message>
<xml_diff>
--- a/src/files/tempPDF/Production.xlsx
+++ b/src/files/tempPDF/Production.xlsx
@@ -11,16 +11,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Édité le : 30/01/2025 à 20:08:38
-  par :</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Édité le : 31/01/2025 à 23:56:46
+Par : FouedAmich</t>
   </si>
   <si>
     <t>Etat Du Production : SOFIEN AMICH</t>
   </si>
   <si>
-    <t>Le : 12/12/2024</t>
+    <t/>
   </si>
   <si>
     <t>Solde exact : 820</t>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>724,00 DT</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>820,00 DT</t>
@@ -199,20 +196,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -220,9 +217,8 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -230,9 +226,8 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -240,9 +235,8 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -250,7 +244,6 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
@@ -297,18 +290,18 @@
         <v>16</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
     <mergeCell ref="A6:A6"/>
     <mergeCell ref="A7:A7"/>
   </mergeCells>

</xml_diff>